<commit_message>
Added code for account and set binary location for chrome
</commit_message>
<xml_diff>
--- a/ReadDataFromExcel/MTN_OrderDetails.xlsx
+++ b/ReadDataFromExcel/MTN_OrderDetails.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="144">
   <si>
     <t>Username</t>
   </si>
@@ -429,6 +429,24 @@
   </si>
   <si>
     <t>test08414@yopmail.com</t>
+  </si>
+  <si>
+    <t>test80554@yopmail.com</t>
+  </si>
+  <si>
+    <t>test42182@yopmail.com</t>
+  </si>
+  <si>
+    <t>C!0ud24@h2Ah</t>
+  </si>
+  <si>
+    <t>test89760@yopmail.com</t>
+  </si>
+  <si>
+    <t>test62492@yopmail.com</t>
+  </si>
+  <si>
+    <t>test44332@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -898,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -906,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>